<commit_message>
React 101 Homework updated.
</commit_message>
<xml_diff>
--- a/REACT/101/101.xlsx
+++ b/REACT/101/101.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\REACT\101\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kazemiraz\Desktop\scores\mft-scores\REACT\101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5004768-7186-463A-BBF3-21B97832A745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="react 101" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>No.</t>
   </si>
@@ -58,12 +57,30 @@
   <si>
     <t>Extra (10)</t>
   </si>
+  <si>
+    <t>Q02</t>
+  </si>
+  <si>
+    <t>Q03</t>
+  </si>
+  <si>
+    <t>H01</t>
+  </si>
+  <si>
+    <t>H02</t>
+  </si>
+  <si>
+    <t>H03</t>
+  </si>
+  <si>
+    <t>H04</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -583,14 +600,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="17.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="5.42578125" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="3" bestFit="1" customWidth="1"/>
@@ -606,19 +623,31 @@
     <col min="16" max="16384" width="8.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -632,7 +661,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:26">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -640,12 +669,26 @@
         <f>(11/15)*10</f>
         <v>7.333333333333333</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="C2" s="18">
+        <f>(10/15)*10</f>
+        <v>6.6666666666666661</v>
+      </c>
+      <c r="D2" s="18">
+        <f>(15/25)*10</f>
+        <v>6</v>
+      </c>
+      <c r="E2" s="18">
+        <v>9</v>
+      </c>
+      <c r="F2" s="18">
+        <v>0</v>
+      </c>
+      <c r="G2" s="18">
+        <v>0</v>
+      </c>
+      <c r="H2" s="18">
+        <v>0</v>
+      </c>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
       <c r="K2" s="18"/>
@@ -657,7 +700,7 @@
       <c r="Q2" s="18"/>
       <c r="R2" s="17">
         <f>SUM(B2:Q2)</f>
-        <v>7.333333333333333</v>
+        <v>29</v>
       </c>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
@@ -668,7 +711,7 @@
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:26">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -676,12 +719,26 @@
         <f>(14/15)*10</f>
         <v>9.3333333333333339</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="C3" s="5">
+        <f>(11/15)*10</f>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="D3" s="5">
+        <f>(23/25)*10</f>
+        <v>9.2000000000000011</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="G3" s="5">
+        <v>9</v>
+      </c>
+      <c r="H3" s="5">
+        <v>9.75</v>
+      </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -692,8 +749,8 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="17">
-        <f t="shared" ref="R3:R12" si="0">SUM(B3:Q3)</f>
-        <v>9.3333333333333339</v>
+        <f>SUM(B3:Q3)</f>
+        <v>54.116666666666667</v>
       </c>
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
@@ -704,7 +761,7 @@
       <c r="Y3" s="6"/>
       <c r="Z3" s="6"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:26">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -712,12 +769,25 @@
         <f>(12/15)*10</f>
         <v>8</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="C4" s="5">
+        <f>(5/15)*10</f>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>9</v>
+      </c>
+      <c r="F4" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -728,8 +798,8 @@
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="17">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f t="shared" ref="R3:R12" si="0">SUM(B4:Q4)</f>
+        <v>29.833333333333332</v>
       </c>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
@@ -740,19 +810,31 @@
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:26">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5">
+        <v>7</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -764,7 +846,7 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
@@ -775,19 +857,31 @@
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:26">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="5">
         <v>0</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -810,7 +904,7 @@
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:26">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -818,12 +912,25 @@
         <f>(15/15)*10</f>
         <v>10</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="C7" s="5">
+        <f>(8/15)*10</f>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>9</v>
+      </c>
+      <c r="F7" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="G7" s="5">
+        <v>9</v>
+      </c>
+      <c r="H7" s="5">
+        <v>8.5</v>
+      </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
@@ -835,7 +942,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="17">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>51.333333333333329</v>
       </c>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
@@ -846,7 +953,7 @@
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:26">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -854,12 +961,25 @@
         <f>(15/15)*10</f>
         <v>10</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="C8" s="5">
+        <f>(13/15)*10</f>
+        <v>8.6666666666666679</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="F8" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -871,7 +991,7 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="17">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>37.666666666666671</v>
       </c>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
@@ -882,7 +1002,7 @@
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:26">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -890,12 +1010,26 @@
         <f>(11/15)*10</f>
         <v>7.333333333333333</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="C9" s="5">
+        <f>(6/15)*10</f>
+        <v>4</v>
+      </c>
+      <c r="D9" s="5">
+        <f>(18/25)*10</f>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
@@ -907,7 +1041,7 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="17">
         <f t="shared" si="0"/>
-        <v>7.333333333333333</v>
+        <v>18.533333333333331</v>
       </c>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
@@ -918,7 +1052,7 @@
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:26">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -926,12 +1060,26 @@
         <f>(15/15)*10</f>
         <v>10</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="C10" s="5">
+        <f>(10/15)*10</f>
+        <v>6.6666666666666661</v>
+      </c>
+      <c r="D10" s="5">
+        <f>(21/25)*10</f>
+        <v>8.4</v>
+      </c>
+      <c r="E10" s="5">
+        <v>9</v>
+      </c>
+      <c r="F10" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="G10" s="5">
+        <v>10</v>
+      </c>
+      <c r="H10" s="5">
+        <v>8.5</v>
+      </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -943,7 +1091,7 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="17">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>62.066666666666663</v>
       </c>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
@@ -954,19 +1102,31 @@
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:26">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="5">
         <v>0</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -989,7 +1149,7 @@
       <c r="Y11" s="6"/>
       <c r="Z11" s="6"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:26">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -997,12 +1157,26 @@
         <f>(14/15)*10</f>
         <v>9.3333333333333339</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="C12" s="5">
+        <f>(13/15)*10</f>
+        <v>8.6666666666666679</v>
+      </c>
+      <c r="D12" s="5">
+        <f>(21/25)*10</f>
+        <v>8.4</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>9</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -1014,7 +1188,7 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="17">
         <f t="shared" si="0"/>
-        <v>9.3333333333333339</v>
+        <v>35.4</v>
       </c>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
@@ -1025,7 +1199,7 @@
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:26">
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -1051,7 +1225,7 @@
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:26">
       <c r="A14" s="7" t="s">
         <v>0</v>
       </c>
@@ -1091,27 +1265,27 @@
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:26">
       <c r="A15" s="7">
         <v>1</v>
       </c>
       <c r="B15" s="10">
         <f>(SUM(B2:Q2)/(COUNTA(B1:Q1) * 10)) * 40</f>
-        <v>29.333333333333332</v>
+        <v>16.571428571428573</v>
       </c>
       <c r="C15" s="11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D15" s="11">
         <v>0</v>
       </c>
       <c r="E15" s="12">
         <f>B15+C15+D15</f>
-        <v>29.333333333333332</v>
+        <v>24.571428571428573</v>
       </c>
       <c r="F15" s="19">
         <f>C15+D15+E15</f>
-        <v>29.333333333333332</v>
+        <v>32.571428571428569</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -1134,27 +1308,27 @@
       <c r="Y15" s="6"/>
       <c r="Z15" s="6"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:26">
       <c r="A16" s="7">
         <v>2</v>
       </c>
       <c r="B16" s="10">
         <f>(SUM(B3:Q3)/(COUNTA(B1:Q1) * 10)) * 40</f>
-        <v>37.333333333333336</v>
+        <v>30.923809523809524</v>
       </c>
       <c r="C16" s="11">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="D16" s="11">
         <v>0</v>
       </c>
       <c r="E16" s="12">
         <f t="shared" ref="E16:F25" si="1">B16+C16+D16</f>
-        <v>37.333333333333336</v>
+        <v>40.423809523809524</v>
       </c>
       <c r="F16" s="19">
         <f t="shared" si="1"/>
-        <v>37.333333333333336</v>
+        <v>49.923809523809524</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -1177,27 +1351,27 @@
       <c r="Y16" s="6"/>
       <c r="Z16" s="6"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:26">
       <c r="A17" s="7">
         <v>3</v>
       </c>
       <c r="B17" s="10">
         <f>(SUM(B4:Q4)/(COUNTA(B1:Q1) * 10)) * 40</f>
-        <v>32</v>
+        <v>17.047619047619047</v>
       </c>
       <c r="C17" s="11">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="D17" s="11">
         <v>0</v>
       </c>
       <c r="E17" s="12">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>25.547619047619047</v>
       </c>
       <c r="F17" s="19">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>34.047619047619051</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -1220,30 +1394,30 @@
       <c r="Y17" s="6"/>
       <c r="Z17" s="6"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:26">
       <c r="A18" s="7">
         <v>4</v>
       </c>
       <c r="B18" s="10">
         <f>(SUM(B5:Q5)/(COUNTA(B1:Q1) * 10)) * 40</f>
-        <v>0</v>
+        <v>8.5714285714285712</v>
       </c>
       <c r="C18" s="11">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D18" s="11">
         <v>0</v>
       </c>
       <c r="E18" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14.571428571428571</v>
       </c>
       <c r="F18" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.45">
+        <v>20.571428571428569</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
       <c r="A19" s="7">
         <v>5</v>
       </c>
@@ -1252,113 +1426,113 @@
         <v>0</v>
       </c>
       <c r="C19" s="11">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D19" s="11">
         <v>0</v>
       </c>
       <c r="E19" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F19" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26">
       <c r="A20" s="7">
         <v>6</v>
       </c>
       <c r="B20" s="10">
         <f>(SUM(B7:Q7)/(COUNTA(B1:Q1) * 10)) * 40</f>
-        <v>40</v>
+        <v>29.333333333333332</v>
       </c>
       <c r="C20" s="11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D20" s="11">
         <v>0</v>
       </c>
       <c r="E20" s="12">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>38.333333333333329</v>
       </c>
       <c r="F20" s="19">
         <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.45">
+        <v>47.333333333333329</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26">
       <c r="A21" s="7">
         <v>7</v>
       </c>
       <c r="B21" s="10">
         <f>(SUM(B8:Q8)/(COUNTA(B1:Q1) * 10)) * 40</f>
-        <v>40</v>
+        <v>21.523809523809526</v>
       </c>
       <c r="C21" s="11">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D21" s="11">
         <v>0</v>
       </c>
       <c r="E21" s="12">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>31.523809523809526</v>
       </c>
       <c r="F21" s="19">
         <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.45">
+        <v>41.523809523809526</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26">
       <c r="A22" s="7">
         <v>8</v>
       </c>
       <c r="B22" s="10">
         <f>(SUM(B9:Q9)/(COUNTA(B1:Q1) * 10)) * 40</f>
-        <v>29.333333333333332</v>
+        <v>10.59047619047619</v>
       </c>
       <c r="C22" s="11">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="D22" s="11">
         <v>0</v>
       </c>
       <c r="E22" s="12">
         <f t="shared" si="1"/>
-        <v>29.333333333333332</v>
+        <v>18.090476190476188</v>
       </c>
       <c r="F22" s="19">
         <f t="shared" si="1"/>
-        <v>29.333333333333332</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.45">
+        <v>25.590476190476188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26">
       <c r="A23" s="7">
         <v>9</v>
       </c>
       <c r="B23" s="10">
         <f>(SUM(B10:Q10)/(COUNTA(B1:Q1) * 10)) * 40</f>
-        <v>40</v>
+        <v>35.466666666666661</v>
       </c>
       <c r="C23" s="11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D23" s="11">
         <v>0</v>
       </c>
       <c r="E23" s="12">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>43.466666666666661</v>
       </c>
       <c r="F23" s="19">
         <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.45">
+        <v>51.466666666666661</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26">
       <c r="A24" s="7">
         <v>10</v>
       </c>
@@ -1367,44 +1541,44 @@
         <v>0</v>
       </c>
       <c r="C24" s="11">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D24" s="11">
         <v>0</v>
       </c>
       <c r="E24" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F24" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26">
       <c r="A25" s="7">
         <v>11</v>
       </c>
       <c r="B25" s="10">
         <f>(SUM(B12:Q12)/(COUNTA(B1:Q1) * 10)) * 40</f>
-        <v>37.333333333333336</v>
+        <v>20.228571428571428</v>
       </c>
       <c r="C25" s="11">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D25" s="11">
         <v>0</v>
       </c>
       <c r="E25" s="12">
         <f t="shared" si="1"/>
-        <v>39.333333333333336</v>
+        <v>29.228571428571428</v>
       </c>
       <c r="F25" s="19">
         <f>C25+D25+E25</f>
-        <v>41.333333333333336</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.45">
+        <v>38.228571428571428</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26">
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1412,7 +1586,7 @@
       <c r="E28" s="15"/>
       <c r="F28" s="16"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:26">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1420,7 +1594,7 @@
       <c r="E29" s="15"/>
       <c r="F29" s="16"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:26">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -1428,7 +1602,7 @@
       <c r="E30" s="15"/>
       <c r="F30" s="16"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:26">
       <c r="A31" s="14"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>

</xml_diff>

<commit_message>
react 101 final scores updated
</commit_message>
<xml_diff>
--- a/REACT/101/101.xlsx
+++ b/REACT/101/101.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kazemiraz\Desktop\scores\mft-scores\REACT\101\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkazemiraz/Desktop/scores/mft-scores/REACT/101/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53327EB-BEAD-5344-9211-B768C0895020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="react 101" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -32,15 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>No.</t>
   </si>
   <si>
     <t>Final Scores</t>
-  </si>
-  <si>
-    <t>MFT</t>
   </si>
   <si>
     <t>Q01</t>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -107,7 +107,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,12 +134,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor rgb="FF993366"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFE699"/>
         <bgColor rgb="FFFFDAA2"/>
       </patternFill>
@@ -154,12 +148,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -180,7 +168,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -195,10 +183,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -207,11 +192,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,27 +588,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" style="13" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="13"/>
-    <col min="12" max="15" width="9.5703125" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="8.5703125" style="3"/>
+    <col min="6" max="6" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5" style="12" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="12" customWidth="1"/>
+    <col min="9" max="9" width="9.5" style="12" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="8.5" style="12"/>
+    <col min="12" max="15" width="9.5" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="8.5" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -628,25 +616,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -658,47 +646,47 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="17">
         <f>(11/15)*10</f>
         <v>7.333333333333333</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="17">
         <f>(10/15)*10</f>
         <v>6.6666666666666661</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="17">
         <f>(15/25)*10</f>
         <v>6</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="17">
         <v>9</v>
       </c>
-      <c r="F2" s="18">
-        <v>0</v>
-      </c>
-      <c r="G2" s="18">
-        <v>0</v>
-      </c>
-      <c r="H2" s="18">
-        <v>0</v>
-      </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="17">
+      <c r="F2" s="17">
+        <v>0</v>
+      </c>
+      <c r="G2" s="17">
+        <v>0</v>
+      </c>
+      <c r="H2" s="17">
+        <v>0</v>
+      </c>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="16">
         <f>SUM(B2:Q2)</f>
         <v>29</v>
       </c>
@@ -748,7 +736,7 @@
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
-      <c r="R3" s="17">
+      <c r="R3" s="16">
         <f>SUM(B3:Q3)</f>
         <v>54.116666666666667</v>
       </c>
@@ -797,8 +785,8 @@
       <c r="O4" s="5"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
-      <c r="R4" s="17">
-        <f t="shared" ref="R3:R12" si="0">SUM(B4:Q4)</f>
+      <c r="R4" s="16">
+        <f t="shared" ref="R4:R12" si="0">SUM(B4:Q4)</f>
         <v>29.833333333333332</v>
       </c>
       <c r="S4" s="6"/>
@@ -844,7 +832,7 @@
       <c r="O5" s="5"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
-      <c r="R5" s="17">
+      <c r="R5" s="16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -891,7 +879,7 @@
       <c r="O6" s="5"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
-      <c r="R6" s="17">
+      <c r="R6" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -940,7 +928,7 @@
       <c r="O7" s="5"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
-      <c r="R7" s="17">
+      <c r="R7" s="16">
         <f t="shared" si="0"/>
         <v>51.333333333333329</v>
       </c>
@@ -989,7 +977,7 @@
       <c r="O8" s="5"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
-      <c r="R8" s="17">
+      <c r="R8" s="16">
         <f t="shared" si="0"/>
         <v>37.666666666666671</v>
       </c>
@@ -1039,7 +1027,7 @@
       <c r="O9" s="5"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
-      <c r="R9" s="17">
+      <c r="R9" s="16">
         <f t="shared" si="0"/>
         <v>18.533333333333331</v>
       </c>
@@ -1089,7 +1077,7 @@
       <c r="O10" s="5"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
-      <c r="R10" s="17">
+      <c r="R10" s="16">
         <f t="shared" si="0"/>
         <v>62.066666666666663</v>
       </c>
@@ -1136,7 +1124,7 @@
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
-      <c r="R11" s="17">
+      <c r="R11" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1186,7 +1174,7 @@
       <c r="O12" s="5"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
-      <c r="R12" s="17">
+      <c r="R12" s="16">
         <f t="shared" si="0"/>
         <v>35.4</v>
       </c>
@@ -1230,20 +1218,18 @@
         <v>0</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>4</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>5</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>2</v>
-      </c>
+      <c r="F14" s="18"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1269,24 +1255,21 @@
       <c r="A15" s="7">
         <v>1</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <f>(SUM(B2:Q2)/(COUNTA(B1:Q1) * 10)) * 40</f>
         <v>16.571428571428573</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="10">
         <v>8</v>
       </c>
-      <c r="D15" s="11">
-        <v>0</v>
-      </c>
-      <c r="E15" s="12">
+      <c r="D15" s="10">
+        <v>45</v>
+      </c>
+      <c r="E15" s="11">
         <f>B15+C15+D15</f>
-        <v>24.571428571428573</v>
-      </c>
-      <c r="F15" s="19">
-        <f>C15+D15+E15</f>
-        <v>32.571428571428569</v>
-      </c>
+        <v>69.571428571428569</v>
+      </c>
+      <c r="F15" s="19"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -1312,24 +1295,21 @@
       <c r="A16" s="7">
         <v>2</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="9">
         <f>(SUM(B3:Q3)/(COUNTA(B1:Q1) * 10)) * 40</f>
         <v>30.923809523809524</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <v>9.5</v>
       </c>
-      <c r="D16" s="11">
-        <v>0</v>
-      </c>
-      <c r="E16" s="12">
+      <c r="D16" s="10">
+        <v>0</v>
+      </c>
+      <c r="E16" s="11">
         <f t="shared" ref="E16:F25" si="1">B16+C16+D16</f>
         <v>40.423809523809524</v>
       </c>
-      <c r="F16" s="19">
-        <f t="shared" si="1"/>
-        <v>49.923809523809524</v>
-      </c>
+      <c r="F16" s="19"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -1355,24 +1335,21 @@
       <c r="A17" s="7">
         <v>3</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <f>(SUM(B4:Q4)/(COUNTA(B1:Q1) * 10)) * 40</f>
         <v>17.047619047619047</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="10">
         <v>8.5</v>
       </c>
-      <c r="D17" s="11">
-        <v>0</v>
-      </c>
-      <c r="E17" s="12">
+      <c r="D17" s="10">
+        <v>50</v>
+      </c>
+      <c r="E17" s="11">
         <f t="shared" si="1"/>
-        <v>25.547619047619047</v>
-      </c>
-      <c r="F17" s="19">
-        <f t="shared" si="1"/>
-        <v>34.047619047619051</v>
-      </c>
+        <v>75.547619047619051</v>
+      </c>
+      <c r="F17" s="19"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1398,217 +1375,193 @@
       <c r="A18" s="7">
         <v>4</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="9">
         <f>(SUM(B5:Q5)/(COUNTA(B1:Q1) * 10)) * 40</f>
         <v>8.5714285714285712</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>6</v>
       </c>
-      <c r="D18" s="11">
-        <v>0</v>
-      </c>
-      <c r="E18" s="12">
+      <c r="D18" s="10">
+        <v>0</v>
+      </c>
+      <c r="E18" s="11">
         <f t="shared" si="1"/>
         <v>14.571428571428571</v>
       </c>
-      <c r="F18" s="19">
-        <f t="shared" si="1"/>
-        <v>20.571428571428569</v>
-      </c>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="1:26">
       <c r="A19" s="7">
         <v>5</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <f>(SUM(B6:Q6)/(COUNTA(B1:Q1) * 10)) * 40</f>
         <v>0</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="10">
         <v>6</v>
       </c>
-      <c r="D19" s="11">
-        <v>0</v>
-      </c>
-      <c r="E19" s="12">
+      <c r="D19" s="10">
+        <v>0</v>
+      </c>
+      <c r="E19" s="11">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F19" s="19">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
+      <c r="F19" s="19"/>
     </row>
     <row r="20" spans="1:26">
       <c r="A20" s="7">
         <v>6</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <f>(SUM(B7:Q7)/(COUNTA(B1:Q1) * 10)) * 40</f>
         <v>29.333333333333332</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="10">
         <v>9</v>
       </c>
-      <c r="D20" s="11">
-        <v>0</v>
-      </c>
-      <c r="E20" s="12">
+      <c r="D20" s="10">
+        <v>50</v>
+      </c>
+      <c r="E20" s="11">
         <f t="shared" si="1"/>
-        <v>38.333333333333329</v>
-      </c>
-      <c r="F20" s="19">
-        <f t="shared" si="1"/>
-        <v>47.333333333333329</v>
-      </c>
+        <v>88.333333333333329</v>
+      </c>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" spans="1:26">
       <c r="A21" s="7">
         <v>7</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <f>(SUM(B8:Q8)/(COUNTA(B1:Q1) * 10)) * 40</f>
         <v>21.523809523809526</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="10">
         <v>10</v>
       </c>
-      <c r="D21" s="11">
-        <v>0</v>
-      </c>
-      <c r="E21" s="12">
+      <c r="D21" s="10">
+        <v>0</v>
+      </c>
+      <c r="E21" s="11">
         <f t="shared" si="1"/>
         <v>31.523809523809526</v>
       </c>
-      <c r="F21" s="19">
-        <f t="shared" si="1"/>
-        <v>41.523809523809526</v>
-      </c>
+      <c r="F21" s="19"/>
     </row>
     <row r="22" spans="1:26">
       <c r="A22" s="7">
         <v>8</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <f>(SUM(B9:Q9)/(COUNTA(B1:Q1) * 10)) * 40</f>
         <v>10.59047619047619</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="10">
         <v>7.5</v>
       </c>
-      <c r="D22" s="11">
-        <v>0</v>
-      </c>
-      <c r="E22" s="12">
+      <c r="D22" s="10">
+        <v>0</v>
+      </c>
+      <c r="E22" s="11">
         <f t="shared" si="1"/>
         <v>18.090476190476188</v>
       </c>
-      <c r="F22" s="19">
-        <f t="shared" si="1"/>
-        <v>25.590476190476188</v>
-      </c>
+      <c r="F22" s="19"/>
     </row>
     <row r="23" spans="1:26">
       <c r="A23" s="7">
         <v>9</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="9">
         <f>(SUM(B10:Q10)/(COUNTA(B1:Q1) * 10)) * 40</f>
         <v>35.466666666666661</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="10">
         <v>8</v>
       </c>
-      <c r="D23" s="11">
-        <v>0</v>
-      </c>
-      <c r="E23" s="12">
+      <c r="D23" s="10">
+        <v>50</v>
+      </c>
+      <c r="E23" s="11">
         <f t="shared" si="1"/>
-        <v>43.466666666666661</v>
-      </c>
-      <c r="F23" s="19">
-        <f t="shared" si="1"/>
-        <v>51.466666666666661</v>
-      </c>
+        <v>93.466666666666669</v>
+      </c>
+      <c r="F23" s="19"/>
     </row>
     <row r="24" spans="1:26">
       <c r="A24" s="7">
         <v>10</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="9">
         <f>(SUM(B11:Q11)/(COUNTA(B1:Q1) * 10)) * 40</f>
         <v>0</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="10">
         <v>6</v>
       </c>
-      <c r="D24" s="11">
-        <v>0</v>
-      </c>
-      <c r="E24" s="12">
+      <c r="D24" s="10">
+        <v>0</v>
+      </c>
+      <c r="E24" s="11">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F24" s="19">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
+      <c r="F24" s="19"/>
     </row>
     <row r="25" spans="1:26">
       <c r="A25" s="7">
         <v>11</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="9">
         <f>(SUM(B12:Q12)/(COUNTA(B1:Q1) * 10)) * 40</f>
         <v>20.228571428571428</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="10">
         <v>9</v>
       </c>
-      <c r="D25" s="11">
-        <v>0</v>
-      </c>
-      <c r="E25" s="12">
+      <c r="D25" s="10">
+        <v>0</v>
+      </c>
+      <c r="E25" s="11">
         <f t="shared" si="1"/>
         <v>29.228571428571428</v>
       </c>
-      <c r="F25" s="19">
-        <f>C25+D25+E25</f>
-        <v>38.228571428571428</v>
-      </c>
+      <c r="F25" s="19"/>
     </row>
     <row r="28" spans="1:26">
-      <c r="A28" s="14"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="16"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="15"/>
     </row>
     <row r="29" spans="1:26">
-      <c r="A29" s="14"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="16"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="15"/>
     </row>
     <row r="30" spans="1:26">
-      <c r="A30" s="14"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="16"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="15"/>
     </row>
     <row r="31" spans="1:26">
-      <c r="A31" s="14"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="16"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>